<commit_message>
add labels to excel proportions
</commit_message>
<xml_diff>
--- a/data/clean/Delphi2_percentages.xlsx
+++ b/data/clean/Delphi2_percentages.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="381" uniqueCount="206">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="476" uniqueCount="301">
   <si>
     <t>cluster</t>
   </si>
@@ -20,6 +20,9 @@
     <t>variable</t>
   </si>
   <si>
+    <t>label</t>
+  </si>
+  <si>
     <t>value</t>
   </si>
   <si>
@@ -627,6 +630,288 @@
   </si>
   <si>
     <t>Q13_3</t>
+  </si>
+  <si>
+    <t>CLUSTER 1  - Informally assess the asylum seeker's level of host culture acculturation.</t>
+  </si>
+  <si>
+    <t>CLUSTER 1  - Belong to the asylum seeker's culture and speak the language.</t>
+  </si>
+  <si>
+    <t>CLUSTER 1  - Avoid excessive culturalisation and a disproportionate emphasis on cultural influences and stereotypes, to the detriment of other important considerations during the conversation.</t>
+  </si>
+  <si>
+    <t>CLUSTER 1  - Acknowledge that cultural backgrounds and societal positions interact in determining mental health experiences.</t>
+  </si>
+  <si>
+    <t>CLUSTER 1  - Be aware that for many asylum seekers there is a strong connection between spirituality and mental health.</t>
+  </si>
+  <si>
+    <t>CLUSTER 1  - Be aware of the wide range of concepts, definitions and idioms of mental health, used by asylum seekers to communicate about their needs.</t>
+  </si>
+  <si>
+    <t>CLUSTER 1  - Encourage an in-depth exchange of views on mental health (care) and be committed to learning about asylum seekers’ views.</t>
+  </si>
+  <si>
+    <t>CLUSTER 1  - Understand and recognise common mental health challenges and their varied manifestations among asylum seekers.</t>
+  </si>
+  <si>
+    <t>CLUSTER 1  - Be aware of ethnocentrism</t>
+  </si>
+  <si>
+    <t>CLUSTER 1  - Demonstrate openness to cultural differences and cultural humility.</t>
+  </si>
+  <si>
+    <t>CLUSTER 1  - Do not cast Western mental health categories as universal, avoiding the category fallacy.</t>
+  </si>
+  <si>
+    <t>CLUSTER 1  - Reflect on the influence and limitations of your own cultural context, views and biases.</t>
+  </si>
+  <si>
+    <t>CLUSTER 1  - Be aware of the unique characteristics of the resident (e.g. ethnic, cultural, spiritual, social, educational, linguistic) and how these may influence mental health conversations.</t>
+  </si>
+  <si>
+    <t>CLUSTER 1  - Be knowledgeable about how cultural backgrounds can shape the understanding, experience and expression of mental health.</t>
+  </si>
+  <si>
+    <t>CLUSTER 1  - Be aware that the use of certain terms and labels can be stigmatising for asylum seekers.</t>
+  </si>
+  <si>
+    <t>CLUSTER 1  - Check the cultural appropriateness of mental health assessment tools and interpret results with caution.</t>
+  </si>
+  <si>
+    <t>CLUSTER 2 - Show your humanity and approach asylum seekers as human beings with struggles, challenges, hopes and dreams similar to your own.</t>
+  </si>
+  <si>
+    <t>CLUSTER 2 - Spend time interacting with asylum seekers to understand their needs.</t>
+  </si>
+  <si>
+    <t>CLUSTER 2 - Demonstrate deep respect for asylum seekers, not judge them.</t>
+  </si>
+  <si>
+    <t>CLUSTER 2 - Look for ways to connect with the asylum seeker to create a basis for the conversation.</t>
+  </si>
+  <si>
+    <t>CLUSTER 2 - Show your willingness and availability to help.</t>
+  </si>
+  <si>
+    <t>CLUSTER 2 - Be compassionate.</t>
+  </si>
+  <si>
+    <t>CLUSTER 2 - Be empathic.</t>
+  </si>
+  <si>
+    <t>CLUSTER 2 - Be curious.</t>
+  </si>
+  <si>
+    <t>CLUSTER 2 - Establish a relationship that promotes safety and builds trust.</t>
+  </si>
+  <si>
+    <t>CLUSTER 2 - Establish rapport and working alliance.</t>
+  </si>
+  <si>
+    <t>CLUSTER 2 - Foster a safe and welcoming environment so that asylum seekers feel valued and understood.</t>
+  </si>
+  <si>
+    <t>CLUSTER 2 - Be trustworthy and honest about your limitations and those of the system in which you operate.</t>
+  </si>
+  <si>
+    <t>CLUSTER 3 - Ask open-ended questions.</t>
+  </si>
+  <si>
+    <t>CLUSTER 3 - Accommodate communicative needs, barriers and limitations by including translators or multilingual colleagues in the conversation.</t>
+  </si>
+  <si>
+    <t>CLUSTER 3 - Listen actively.</t>
+  </si>
+  <si>
+    <t>CLUSTER 3 - Be aware of language nuances and that things can get lost in translation.</t>
+  </si>
+  <si>
+    <t>CLUSTER 3 - Conduct mental health conversations at a pace that is comfortable and tolerable for asylum seekers.</t>
+  </si>
+  <si>
+    <t>CLUSTER 3 - Pay attention to non-verbal communication.</t>
+  </si>
+  <si>
+    <t>CLUSTER 3 - Adapt your communication style to suit the person and the situation at hand.</t>
+  </si>
+  <si>
+    <t>CLUSTER 4 - Take the lead from asylum seekers.</t>
+  </si>
+  <si>
+    <t>CLUSTER 4 - Be committed to identifying and working with asylum seekers' preferred approaches and resources for managing mental health and reducing distress.</t>
+  </si>
+  <si>
+    <t>CLUSTER 4 - Know that some behaviours require immediate professional attention to save lives.</t>
+  </si>
+  <si>
+    <t>CLUSTER 4 - Centre the asylum seekers' voices and the priorities they highlight during the conversation, accepting that they may be different from your own.</t>
+  </si>
+  <si>
+    <t>CLUSTER 4 - Respond to immediate concerns.</t>
+  </si>
+  <si>
+    <t>CLUSTER 4 - Avoid imposing your own views and approaches on asylum seekers.</t>
+  </si>
+  <si>
+    <t>CLUSTER 5 - Encourage and enable asylum seekers to sustain existing relationships.</t>
+  </si>
+  <si>
+    <t>CLUSTER 5 - Know the wide range of mental health resources and how to promote resilience.</t>
+  </si>
+  <si>
+    <t>CLUSTER 5 - Approach the conversation from a strength (resilience) perspective to address feelings of powerlessness and helplessness.</t>
+  </si>
+  <si>
+    <t>CLUSTER 5 - Build a bridge between the asylum seeker's perspective and experiences and the resources and services available.</t>
+  </si>
+  <si>
+    <t>CLUSTER 5 - Explore what has sustained the asylum seekers through their experiences and identify together how they can continue to use and build on these resources.</t>
+  </si>
+  <si>
+    <t>CLUSTER 5 - Facilitate connections with relevant community resources and support networks, aiding in the integration and social support of residents.</t>
+  </si>
+  <si>
+    <t>CLUSTER 6 - Initiate scalable psychological interventions.</t>
+  </si>
+  <si>
+    <t>CLUSTER 6 - Provide psychological first aid.</t>
+  </si>
+  <si>
+    <t>CLUSTER 6 - Adopt a survivor-centred approach.</t>
+  </si>
+  <si>
+    <t>CLUSTER 6 - Adopt a trauma-informed approach.</t>
+  </si>
+  <si>
+    <t>CLUSTER 6 - Be aware that mindfulness practices can help to gain some control over emotions.</t>
+  </si>
+  <si>
+    <t>CLUSTER 6 - Blend insights and approaches from diverse cultures in ways that promote well-being.</t>
+  </si>
+  <si>
+    <t>CLUSTER 6 - Employ de-escalation techniques and support emotional regulation.</t>
+  </si>
+  <si>
+    <t>CLUSTER 6 - Know how to help prevent gender-based violence and child protection violations.</t>
+  </si>
+  <si>
+    <t>CLUSTER 6 - Pay attention to mind-body connections and psychosomatic experiences and expressions.</t>
+  </si>
+  <si>
+    <t>CLUSTER 6 - Understand the importance of family and a collective approach to help seeking.</t>
+  </si>
+  <si>
+    <t>CLUSTER 6 - Know that even short conversations can be very significant.</t>
+  </si>
+  <si>
+    <t>CLUSTER 6 - Provide assistance with practical challenges and accompany asylum seekers in meeting requirements.</t>
+  </si>
+  <si>
+    <t>CLUSTER 6 - Implement protocols, approaches and interventions that are sensitive to cultural differences among asylum seekers.</t>
+  </si>
+  <si>
+    <t>CLUSTER 6 - Contextualise and normalise asylum seekers' mental health presentations, taking into account their specific situation and unique context.</t>
+  </si>
+  <si>
+    <t>CLUSTER 7 - Realise that asylum seekers are typically struggling with a series of practical challenges that they need to solve before they are ready to address their mental health issues.</t>
+  </si>
+  <si>
+    <t>CLUSTER 7 - Realise that the organisational context and characteristics influence mental health conversations with asylum seekers.</t>
+  </si>
+  <si>
+    <t>CLUSTER 7 - Recognise that asylum applications and procedures evoke strong emotions.</t>
+  </si>
+  <si>
+    <t>CLUSTER 7 - Consider pre-, peri- and post-migration stressors and their impact on mental health.</t>
+  </si>
+  <si>
+    <t>CLUSTER 7 - Be familiar with the basics of the asylum policy and procedure and have resources to help asylum seekers find answers to their questions.</t>
+  </si>
+  <si>
+    <t>CLUSTER 7 - Keep in mind that asylum seekers may have had to tell their story many times, sometimes in hostile circumstances.</t>
+  </si>
+  <si>
+    <t>CLUSTER 7 - Realise that systemic and structural factors influence an individual's mental health capacity and needs.</t>
+  </si>
+  <si>
+    <t>CLUSTER 7 - Have an understanding of the context of displacement and (forced) migration, the kinds of situations that asylum seekers are likely to have been exposed to and how this may impact on mental health.</t>
+  </si>
+  <si>
+    <t>CLUSTER 7 - Understand that current living conditions and experiences can trigger and exacerbate mental health challenges.</t>
+  </si>
+  <si>
+    <t>CLUSTER 8 - Express support for the resident’s asylum claim.</t>
+  </si>
+  <si>
+    <t>CLUSTER 8 - Recognise and resist oppressive government policies and measures.</t>
+  </si>
+  <si>
+    <t>CLUSTER 8 - Mitigate power inequalities in the relationship and show your commitment to equity.</t>
+  </si>
+  <si>
+    <t>CLUSTER 8 - Safeguard human rights and social justice.</t>
+  </si>
+  <si>
+    <t>CLUSTER 8 - Identify and acknowledge injustices faced by asylum seekers.</t>
+  </si>
+  <si>
+    <t>CLUSTER 8 - Identify barriers that may prevent asylum seekers from benefiting from particular approaches, interventions and treatments.</t>
+  </si>
+  <si>
+    <t>CLUSTER 9 - Tolerate feelings of powerlessness and helplessness due to lack of immediate solutions.</t>
+  </si>
+  <si>
+    <t>CLUSTER 9 - Be aware of the fact that this work implicitly or explicitly has an impact on the way you perceive political debate.</t>
+  </si>
+  <si>
+    <t>CLUSTER 9 - Be prepared to tolerate strong emotions.</t>
+  </si>
+  <si>
+    <t>CLUSTER 9 - Engage in self-care and well-being practices, to take care of your own mental health.</t>
+  </si>
+  <si>
+    <t>CLUSTER 9 - Commit to ongoing professional development, be open to learning from your work and to be supported in reflecting on your mental health conversations with asylum seekers.</t>
+  </si>
+  <si>
+    <t>CLUSTER 9 - Reflect on the influence of your own life history and experiences.</t>
+  </si>
+  <si>
+    <t>CLUSTER 9 - Be mindful of not abusing your power.</t>
+  </si>
+  <si>
+    <t>CLUSTER 10 - Collaborate with peer workers who share lived experiences with the residents.</t>
+  </si>
+  <si>
+    <t>CLUSTER 10 - Collaborate with people who can provide experience-based insights into cultural meanings and understandings of mental health.</t>
+  </si>
+  <si>
+    <t>CLUSTER 10 - Work in a network that addresses different areas of life, in the knowledge that a holistic, multi-sectoral approach is essential.</t>
+  </si>
+  <si>
+    <t>CLUSTER 10 - Navigate available services and know when and where to orientate asylum seekers in need of additional support.</t>
+  </si>
+  <si>
+    <t>CLUSTER 11 - Be willing to bend and defy rules and regulations.</t>
+  </si>
+  <si>
+    <t>CLUSTER 11 - Check the asylum seekers’ consent to talk about certain issues, understanding that they may face barriers to having mental health conversations and disclosing mental health needs.</t>
+  </si>
+  <si>
+    <t>CLUSTER 11 - Communicate clearly about confidentiality and be transparent about its limits.</t>
+  </si>
+  <si>
+    <t>CLUSTER 11 - Respect the imperative of "do no harm" and the principles of ethical conduct.</t>
+  </si>
+  <si>
+    <t>CLUSTER 12 - Avoid eliciting detailed recounts of past experiences, and instead focus on the impact and resulting needs.</t>
+  </si>
+  <si>
+    <t>CLUSTER 12 - Understand that trauma affects memory and can lead to inconsistent narratives from asylum seekers.</t>
+  </si>
+  <si>
+    <t>CLUSTER 12 - Choose a place for the conversations that feels safe to the asylum seeker.</t>
   </si>
   <si>
     <t>I agree</t>
@@ -697,1884 +982,2169 @@
       <c r="F1" t="s">
         <v>4</v>
       </c>
+      <c r="G1" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C2" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="D2" t="s">
-        <v>205</v>
-      </c>
-      <c r="E2" t="n">
+        <v>206</v>
+      </c>
+      <c r="E2" t="s">
+        <v>300</v>
+      </c>
+      <c r="F2" t="n">
         <v>11.0</v>
       </c>
-      <c r="F2" t="n">
+      <c r="G2" t="n">
         <v>0.4230769230769231</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B3" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C3" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="D3" t="s">
-        <v>205</v>
-      </c>
-      <c r="E3" t="n">
+        <v>207</v>
+      </c>
+      <c r="E3" t="s">
+        <v>300</v>
+      </c>
+      <c r="F3" t="n">
         <v>4.0</v>
       </c>
-      <c r="F3" t="n">
+      <c r="G3" t="n">
         <v>0.15384615384615385</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B4" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C4" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="D4" t="s">
-        <v>205</v>
-      </c>
-      <c r="E4" t="n">
+        <v>208</v>
+      </c>
+      <c r="E4" t="s">
+        <v>300</v>
+      </c>
+      <c r="F4" t="n">
         <v>16.0</v>
       </c>
-      <c r="F4" t="n">
+      <c r="G4" t="n">
         <v>0.6153846153846154</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B5" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C5" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="D5" t="s">
-        <v>205</v>
-      </c>
-      <c r="E5" t="n">
+        <v>209</v>
+      </c>
+      <c r="E5" t="s">
+        <v>300</v>
+      </c>
+      <c r="F5" t="n">
         <v>20.0</v>
       </c>
-      <c r="F5" t="n">
+      <c r="G5" t="n">
         <v>0.7407407407407407</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B6" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C6" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="D6" t="s">
-        <v>205</v>
-      </c>
-      <c r="E6" t="n">
+        <v>210</v>
+      </c>
+      <c r="E6" t="s">
+        <v>300</v>
+      </c>
+      <c r="F6" t="n">
         <v>20.0</v>
       </c>
-      <c r="F6" t="n">
+      <c r="G6" t="n">
         <v>0.7692307692307693</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B7" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C7" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="D7" t="s">
-        <v>205</v>
-      </c>
-      <c r="E7" t="n">
+        <v>211</v>
+      </c>
+      <c r="E7" t="s">
+        <v>300</v>
+      </c>
+      <c r="F7" t="n">
         <v>21.0</v>
       </c>
-      <c r="F7" t="n">
+      <c r="G7" t="n">
         <v>0.8076923076923077</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B8" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C8" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="D8" t="s">
-        <v>205</v>
-      </c>
-      <c r="E8" t="n">
+        <v>212</v>
+      </c>
+      <c r="E8" t="s">
+        <v>300</v>
+      </c>
+      <c r="F8" t="n">
         <v>22.0</v>
       </c>
-      <c r="F8" t="n">
+      <c r="G8" t="n">
         <v>0.8461538461538461</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B9" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C9" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="D9" t="s">
-        <v>205</v>
-      </c>
-      <c r="E9" t="n">
+        <v>213</v>
+      </c>
+      <c r="E9" t="s">
+        <v>300</v>
+      </c>
+      <c r="F9" t="n">
         <v>22.0</v>
       </c>
-      <c r="F9" t="n">
+      <c r="G9" t="n">
         <v>0.8461538461538461</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B10" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C10" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="D10" t="s">
-        <v>205</v>
-      </c>
-      <c r="E10" t="n">
+        <v>214</v>
+      </c>
+      <c r="E10" t="s">
+        <v>300</v>
+      </c>
+      <c r="F10" t="n">
         <v>22.0</v>
       </c>
-      <c r="F10" t="n">
+      <c r="G10" t="n">
         <v>0.8461538461538461</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B11" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C11" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="D11" t="s">
-        <v>205</v>
-      </c>
-      <c r="E11" t="n">
+        <v>215</v>
+      </c>
+      <c r="E11" t="s">
+        <v>300</v>
+      </c>
+      <c r="F11" t="n">
         <v>23.0</v>
       </c>
-      <c r="F11" t="n">
+      <c r="G11" t="n">
         <v>0.8846153846153846</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B12" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C12" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="D12" t="s">
-        <v>205</v>
-      </c>
-      <c r="E12" t="n">
+        <v>216</v>
+      </c>
+      <c r="E12" t="s">
+        <v>300</v>
+      </c>
+      <c r="F12" t="n">
         <v>23.0</v>
       </c>
-      <c r="F12" t="n">
+      <c r="G12" t="n">
         <v>0.8846153846153846</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B13" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C13" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="D13" t="s">
-        <v>205</v>
-      </c>
-      <c r="E13" t="n">
+        <v>217</v>
+      </c>
+      <c r="E13" t="s">
+        <v>300</v>
+      </c>
+      <c r="F13" t="n">
         <v>23.0</v>
       </c>
-      <c r="F13" t="n">
+      <c r="G13" t="n">
         <v>0.8846153846153846</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B14" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C14" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="D14" t="s">
-        <v>205</v>
-      </c>
-      <c r="E14" t="n">
+        <v>218</v>
+      </c>
+      <c r="E14" t="s">
+        <v>300</v>
+      </c>
+      <c r="F14" t="n">
         <v>23.0</v>
       </c>
-      <c r="F14" t="n">
+      <c r="G14" t="n">
         <v>0.8846153846153846</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B15" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C15" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="D15" t="s">
-        <v>205</v>
-      </c>
-      <c r="E15" t="n">
+        <v>219</v>
+      </c>
+      <c r="E15" t="s">
+        <v>300</v>
+      </c>
+      <c r="F15" t="n">
         <v>23.0</v>
       </c>
-      <c r="F15" t="n">
+      <c r="G15" t="n">
         <v>0.8846153846153846</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B16" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C16" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="D16" t="s">
-        <v>205</v>
-      </c>
-      <c r="E16" t="n">
+        <v>220</v>
+      </c>
+      <c r="E16" t="s">
+        <v>300</v>
+      </c>
+      <c r="F16" t="n">
         <v>24.0</v>
       </c>
-      <c r="F16" t="n">
+      <c r="G16" t="n">
         <v>0.9230769230769231</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B17" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C17" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="D17" t="s">
-        <v>205</v>
-      </c>
-      <c r="E17" t="n">
+        <v>221</v>
+      </c>
+      <c r="E17" t="s">
+        <v>300</v>
+      </c>
+      <c r="F17" t="n">
         <v>25.0</v>
       </c>
-      <c r="F17" t="n">
+      <c r="G17" t="n">
         <v>0.9615384615384616</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B18" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C18" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="D18" t="s">
-        <v>205</v>
-      </c>
-      <c r="E18" t="n">
+        <v>222</v>
+      </c>
+      <c r="E18" t="s">
+        <v>300</v>
+      </c>
+      <c r="F18" t="n">
         <v>20.0</v>
       </c>
-      <c r="F18" t="n">
+      <c r="G18" t="n">
         <v>0.7407407407407407</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B19" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C19" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="D19" t="s">
-        <v>205</v>
-      </c>
-      <c r="E19" t="n">
+        <v>223</v>
+      </c>
+      <c r="E19" t="s">
+        <v>300</v>
+      </c>
+      <c r="F19" t="n">
         <v>20.0</v>
       </c>
-      <c r="F19" t="n">
+      <c r="G19" t="n">
         <v>0.7407407407407407</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B20" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C20" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="D20" t="s">
-        <v>205</v>
-      </c>
-      <c r="E20" t="n">
+        <v>224</v>
+      </c>
+      <c r="E20" t="s">
+        <v>300</v>
+      </c>
+      <c r="F20" t="n">
         <v>22.0</v>
       </c>
-      <c r="F20" t="n">
+      <c r="G20" t="n">
         <v>0.8148148148148148</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B21" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C21" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="D21" t="s">
-        <v>205</v>
-      </c>
-      <c r="E21" t="n">
+        <v>225</v>
+      </c>
+      <c r="E21" t="s">
+        <v>300</v>
+      </c>
+      <c r="F21" t="n">
         <v>22.0</v>
       </c>
-      <c r="F21" t="n">
+      <c r="G21" t="n">
         <v>0.8148148148148148</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B22" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C22" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="D22" t="s">
-        <v>205</v>
-      </c>
-      <c r="E22" t="n">
+        <v>226</v>
+      </c>
+      <c r="E22" t="s">
+        <v>300</v>
+      </c>
+      <c r="F22" t="n">
         <v>23.0</v>
       </c>
-      <c r="F22" t="n">
+      <c r="G22" t="n">
         <v>0.8518518518518519</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B23" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C23" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="D23" t="s">
-        <v>205</v>
-      </c>
-      <c r="E23" t="n">
+        <v>227</v>
+      </c>
+      <c r="E23" t="s">
+        <v>300</v>
+      </c>
+      <c r="F23" t="n">
         <v>25.0</v>
       </c>
-      <c r="F23" t="n">
+      <c r="G23" t="n">
         <v>0.9259259259259259</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B24" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C24" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="D24" t="s">
-        <v>205</v>
-      </c>
-      <c r="E24" t="n">
+        <v>228</v>
+      </c>
+      <c r="E24" t="s">
+        <v>300</v>
+      </c>
+      <c r="F24" t="n">
         <v>25.0</v>
       </c>
-      <c r="F24" t="n">
+      <c r="G24" t="n">
         <v>0.9259259259259259</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B25" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C25" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="D25" t="s">
-        <v>205</v>
-      </c>
-      <c r="E25" t="n">
+        <v>229</v>
+      </c>
+      <c r="E25" t="s">
+        <v>300</v>
+      </c>
+      <c r="F25" t="n">
         <v>26.0</v>
       </c>
-      <c r="F25" t="n">
+      <c r="G25" t="n">
         <v>0.9629629629629629</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B26" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C26" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="D26" t="s">
-        <v>205</v>
-      </c>
-      <c r="E26" t="n">
+        <v>230</v>
+      </c>
+      <c r="E26" t="s">
+        <v>300</v>
+      </c>
+      <c r="F26" t="n">
         <v>26.0</v>
       </c>
-      <c r="F26" t="n">
+      <c r="G26" t="n">
         <v>0.9629629629629629</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B27" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C27" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="D27" t="s">
-        <v>205</v>
-      </c>
-      <c r="E27" t="n">
+        <v>231</v>
+      </c>
+      <c r="E27" t="s">
+        <v>300</v>
+      </c>
+      <c r="F27" t="n">
         <v>26.0</v>
       </c>
-      <c r="F27" t="n">
+      <c r="G27" t="n">
         <v>0.9629629629629629</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B28" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C28" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="D28" t="s">
-        <v>205</v>
-      </c>
-      <c r="E28" t="n">
+        <v>232</v>
+      </c>
+      <c r="E28" t="s">
+        <v>300</v>
+      </c>
+      <c r="F28" t="n">
         <v>26.0</v>
       </c>
-      <c r="F28" t="n">
+      <c r="G28" t="n">
         <v>0.9629629629629629</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B29" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C29" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="D29" t="s">
-        <v>205</v>
-      </c>
-      <c r="E29" t="n">
+        <v>233</v>
+      </c>
+      <c r="E29" t="s">
+        <v>300</v>
+      </c>
+      <c r="F29" t="n">
         <v>27.0</v>
       </c>
-      <c r="F29" t="n">
+      <c r="G29" t="n">
         <v>1.0</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B30" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C30" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="D30" t="s">
-        <v>205</v>
-      </c>
-      <c r="E30" t="n">
+        <v>234</v>
+      </c>
+      <c r="E30" t="s">
+        <v>300</v>
+      </c>
+      <c r="F30" t="n">
         <v>19.0</v>
       </c>
-      <c r="F30" t="n">
+      <c r="G30" t="n">
         <v>0.7037037037037037</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B31" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C31" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="D31" t="s">
-        <v>205</v>
-      </c>
-      <c r="E31" t="n">
+        <v>235</v>
+      </c>
+      <c r="E31" t="s">
+        <v>300</v>
+      </c>
+      <c r="F31" t="n">
         <v>22.0</v>
       </c>
-      <c r="F31" t="n">
+      <c r="G31" t="n">
         <v>0.8148148148148148</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B32" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C32" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="D32" t="s">
-        <v>205</v>
-      </c>
-      <c r="E32" t="n">
+        <v>236</v>
+      </c>
+      <c r="E32" t="s">
+        <v>300</v>
+      </c>
+      <c r="F32" t="n">
         <v>22.0</v>
       </c>
-      <c r="F32" t="n">
+      <c r="G32" t="n">
         <v>0.8148148148148148</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B33" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C33" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="D33" t="s">
-        <v>205</v>
-      </c>
-      <c r="E33" t="n">
+        <v>237</v>
+      </c>
+      <c r="E33" t="s">
+        <v>300</v>
+      </c>
+      <c r="F33" t="n">
         <v>23.0</v>
       </c>
-      <c r="F33" t="n">
+      <c r="G33" t="n">
         <v>0.8518518518518519</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B34" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C34" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="D34" t="s">
-        <v>205</v>
-      </c>
-      <c r="E34" t="n">
+        <v>238</v>
+      </c>
+      <c r="E34" t="s">
+        <v>300</v>
+      </c>
+      <c r="F34" t="n">
         <v>24.0</v>
       </c>
-      <c r="F34" t="n">
+      <c r="G34" t="n">
         <v>0.8888888888888888</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B35" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C35" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="D35" t="s">
-        <v>205</v>
-      </c>
-      <c r="E35" t="n">
+        <v>239</v>
+      </c>
+      <c r="E35" t="s">
+        <v>300</v>
+      </c>
+      <c r="F35" t="n">
         <v>26.0</v>
       </c>
-      <c r="F35" t="n">
+      <c r="G35" t="n">
         <v>0.9629629629629629</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B36" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C36" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="D36" t="s">
-        <v>205</v>
-      </c>
-      <c r="E36" t="n">
+        <v>240</v>
+      </c>
+      <c r="E36" t="s">
+        <v>300</v>
+      </c>
+      <c r="F36" t="n">
         <v>26.0</v>
       </c>
-      <c r="F36" t="n">
+      <c r="G36" t="n">
         <v>0.9629629629629629</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B37" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C37" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="D37" t="s">
-        <v>205</v>
-      </c>
-      <c r="E37" t="n">
+        <v>241</v>
+      </c>
+      <c r="E37" t="s">
+        <v>300</v>
+      </c>
+      <c r="F37" t="n">
         <v>8.0</v>
       </c>
-      <c r="F37" t="n">
+      <c r="G37" t="n">
         <v>0.2962962962962963</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B38" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C38" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="D38" t="s">
-        <v>205</v>
-      </c>
-      <c r="E38" t="n">
+        <v>242</v>
+      </c>
+      <c r="E38" t="s">
+        <v>300</v>
+      </c>
+      <c r="F38" t="n">
         <v>21.0</v>
       </c>
-      <c r="F38" t="n">
+      <c r="G38" t="n">
         <v>0.7777777777777778</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B39" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C39" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="D39" t="s">
-        <v>205</v>
-      </c>
-      <c r="E39" t="n">
+        <v>243</v>
+      </c>
+      <c r="E39" t="s">
+        <v>300</v>
+      </c>
+      <c r="F39" t="n">
         <v>21.0</v>
       </c>
-      <c r="F39" t="n">
+      <c r="G39" t="n">
         <v>0.7777777777777778</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B40" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C40" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="D40" t="s">
-        <v>205</v>
-      </c>
-      <c r="E40" t="n">
+        <v>244</v>
+      </c>
+      <c r="E40" t="s">
+        <v>300</v>
+      </c>
+      <c r="F40" t="n">
         <v>22.0</v>
       </c>
-      <c r="F40" t="n">
+      <c r="G40" t="n">
         <v>0.8148148148148148</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B41" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C41" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="D41" t="s">
-        <v>205</v>
-      </c>
-      <c r="E41" t="n">
+        <v>245</v>
+      </c>
+      <c r="E41" t="s">
+        <v>300</v>
+      </c>
+      <c r="F41" t="n">
         <v>22.0</v>
       </c>
-      <c r="F41" t="n">
+      <c r="G41" t="n">
         <v>0.8148148148148148</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B42" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C42" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="D42" t="s">
-        <v>205</v>
-      </c>
-      <c r="E42" t="n">
+        <v>246</v>
+      </c>
+      <c r="E42" t="s">
+        <v>300</v>
+      </c>
+      <c r="F42" t="n">
         <v>24.0</v>
       </c>
-      <c r="F42" t="n">
+      <c r="G42" t="n">
         <v>0.8888888888888888</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B43" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C43" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="D43" t="s">
-        <v>205</v>
-      </c>
-      <c r="E43" t="n">
+        <v>247</v>
+      </c>
+      <c r="E43" t="s">
+        <v>300</v>
+      </c>
+      <c r="F43" t="n">
         <v>18.0</v>
       </c>
-      <c r="F43" t="n">
+      <c r="G43" t="n">
         <v>0.6923076923076923</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B44" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C44" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="D44" t="s">
-        <v>205</v>
-      </c>
-      <c r="E44" t="n">
+        <v>248</v>
+      </c>
+      <c r="E44" t="s">
+        <v>300</v>
+      </c>
+      <c r="F44" t="n">
         <v>18.0</v>
       </c>
-      <c r="F44" t="n">
+      <c r="G44" t="n">
         <v>0.6923076923076923</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B45" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C45" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="D45" t="s">
-        <v>205</v>
-      </c>
-      <c r="E45" t="n">
+        <v>249</v>
+      </c>
+      <c r="E45" t="s">
+        <v>300</v>
+      </c>
+      <c r="F45" t="n">
         <v>19.0</v>
       </c>
-      <c r="F45" t="n">
+      <c r="G45" t="n">
         <v>0.7307692307692307</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B46" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C46" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="D46" t="s">
-        <v>205</v>
-      </c>
-      <c r="E46" t="n">
+        <v>250</v>
+      </c>
+      <c r="E46" t="s">
+        <v>300</v>
+      </c>
+      <c r="F46" t="n">
         <v>24.0</v>
       </c>
-      <c r="F46" t="n">
+      <c r="G46" t="n">
         <v>0.9230769230769231</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B47" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C47" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="D47" t="s">
-        <v>205</v>
-      </c>
-      <c r="E47" t="n">
+        <v>251</v>
+      </c>
+      <c r="E47" t="s">
+        <v>300</v>
+      </c>
+      <c r="F47" t="n">
         <v>25.0</v>
       </c>
-      <c r="F47" t="n">
+      <c r="G47" t="n">
         <v>0.9615384615384616</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B48" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C48" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="D48" t="s">
-        <v>205</v>
-      </c>
-      <c r="E48" t="n">
+        <v>252</v>
+      </c>
+      <c r="E48" t="s">
+        <v>300</v>
+      </c>
+      <c r="F48" t="n">
         <v>25.0</v>
       </c>
-      <c r="F48" t="n">
+      <c r="G48" t="n">
         <v>0.9615384615384616</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B49" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="C49" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="D49" t="s">
-        <v>205</v>
-      </c>
-      <c r="E49" t="n">
+        <v>253</v>
+      </c>
+      <c r="E49" t="s">
+        <v>300</v>
+      </c>
+      <c r="F49" t="n">
         <v>13.0</v>
       </c>
-      <c r="F49" t="n">
+      <c r="G49" t="n">
         <v>0.5</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B50" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="C50" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="D50" t="s">
-        <v>205</v>
-      </c>
-      <c r="E50" t="n">
+        <v>254</v>
+      </c>
+      <c r="E50" t="s">
+        <v>300</v>
+      </c>
+      <c r="F50" t="n">
         <v>14.0</v>
       </c>
-      <c r="F50" t="n">
+      <c r="G50" t="n">
         <v>0.5384615384615384</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B51" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="C51" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="D51" t="s">
-        <v>205</v>
-      </c>
-      <c r="E51" t="n">
+        <v>255</v>
+      </c>
+      <c r="E51" t="s">
+        <v>300</v>
+      </c>
+      <c r="F51" t="n">
         <v>16.0</v>
       </c>
-      <c r="F51" t="n">
+      <c r="G51" t="n">
         <v>0.6153846153846154</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B52" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="C52" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="D52" t="s">
-        <v>205</v>
-      </c>
-      <c r="E52" t="n">
+        <v>256</v>
+      </c>
+      <c r="E52" t="s">
+        <v>300</v>
+      </c>
+      <c r="F52" t="n">
         <v>16.0</v>
       </c>
-      <c r="F52" t="n">
+      <c r="G52" t="n">
         <v>0.6153846153846154</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B53" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="C53" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="D53" t="s">
-        <v>205</v>
-      </c>
-      <c r="E53" t="n">
+        <v>257</v>
+      </c>
+      <c r="E53" t="s">
+        <v>300</v>
+      </c>
+      <c r="F53" t="n">
         <v>19.0</v>
       </c>
-      <c r="F53" t="n">
+      <c r="G53" t="n">
         <v>0.7307692307692307</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B54" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="C54" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="D54" t="s">
-        <v>205</v>
-      </c>
-      <c r="E54" t="n">
+        <v>258</v>
+      </c>
+      <c r="E54" t="s">
+        <v>300</v>
+      </c>
+      <c r="F54" t="n">
         <v>19.0</v>
       </c>
-      <c r="F54" t="n">
+      <c r="G54" t="n">
         <v>0.7307692307692307</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B55" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="C55" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="D55" t="s">
-        <v>205</v>
-      </c>
-      <c r="E55" t="n">
+        <v>259</v>
+      </c>
+      <c r="E55" t="s">
+        <v>300</v>
+      </c>
+      <c r="F55" t="n">
         <v>20.0</v>
       </c>
-      <c r="F55" t="n">
+      <c r="G55" t="n">
         <v>0.7692307692307693</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B56" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="C56" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="D56" t="s">
-        <v>205</v>
-      </c>
-      <c r="E56" t="n">
+        <v>260</v>
+      </c>
+      <c r="E56" t="s">
+        <v>300</v>
+      </c>
+      <c r="F56" t="n">
         <v>20.0</v>
       </c>
-      <c r="F56" t="n">
+      <c r="G56" t="n">
         <v>0.7692307692307693</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B57" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="C57" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="D57" t="s">
-        <v>205</v>
-      </c>
-      <c r="E57" t="n">
+        <v>261</v>
+      </c>
+      <c r="E57" t="s">
+        <v>300</v>
+      </c>
+      <c r="F57" t="n">
         <v>22.0</v>
       </c>
-      <c r="F57" t="n">
+      <c r="G57" t="n">
         <v>0.8461538461538461</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B58" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="C58" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="D58" t="s">
-        <v>205</v>
-      </c>
-      <c r="E58" t="n">
+        <v>262</v>
+      </c>
+      <c r="E58" t="s">
+        <v>300</v>
+      </c>
+      <c r="F58" t="n">
         <v>22.0</v>
       </c>
-      <c r="F58" t="n">
+      <c r="G58" t="n">
         <v>0.88</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B59" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="C59" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="D59" t="s">
-        <v>205</v>
-      </c>
-      <c r="E59" t="n">
+        <v>263</v>
+      </c>
+      <c r="E59" t="s">
+        <v>300</v>
+      </c>
+      <c r="F59" t="n">
         <v>23.0</v>
       </c>
-      <c r="F59" t="n">
+      <c r="G59" t="n">
         <v>0.8846153846153846</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B60" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="C60" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="D60" t="s">
-        <v>205</v>
-      </c>
-      <c r="E60" t="n">
+        <v>264</v>
+      </c>
+      <c r="E60" t="s">
+        <v>300</v>
+      </c>
+      <c r="F60" t="n">
         <v>23.0</v>
       </c>
-      <c r="F60" t="n">
+      <c r="G60" t="n">
         <v>0.8846153846153846</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B61" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="C61" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="D61" t="s">
-        <v>205</v>
-      </c>
-      <c r="E61" t="n">
+        <v>265</v>
+      </c>
+      <c r="E61" t="s">
+        <v>300</v>
+      </c>
+      <c r="F61" t="n">
         <v>24.0</v>
       </c>
-      <c r="F61" t="n">
+      <c r="G61" t="n">
         <v>0.9230769230769231</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B62" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="C62" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="D62" t="s">
-        <v>205</v>
-      </c>
-      <c r="E62" t="n">
+        <v>266</v>
+      </c>
+      <c r="E62" t="s">
+        <v>300</v>
+      </c>
+      <c r="F62" t="n">
         <v>25.0</v>
       </c>
-      <c r="F62" t="n">
+      <c r="G62" t="n">
         <v>0.9615384615384616</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B63" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="C63" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="D63" t="s">
-        <v>205</v>
-      </c>
-      <c r="E63" t="n">
+        <v>267</v>
+      </c>
+      <c r="E63" t="s">
+        <v>300</v>
+      </c>
+      <c r="F63" t="n">
         <v>19.0</v>
       </c>
-      <c r="F63" t="n">
+      <c r="G63" t="n">
         <v>0.7307692307692307</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B64" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="C64" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="D64" t="s">
-        <v>205</v>
-      </c>
-      <c r="E64" t="n">
+        <v>268</v>
+      </c>
+      <c r="E64" t="s">
+        <v>300</v>
+      </c>
+      <c r="F64" t="n">
         <v>21.0</v>
       </c>
-      <c r="F64" t="n">
+      <c r="G64" t="n">
         <v>0.8076923076923077</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B65" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="C65" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="D65" t="s">
-        <v>205</v>
-      </c>
-      <c r="E65" t="n">
+        <v>269</v>
+      </c>
+      <c r="E65" t="s">
+        <v>300</v>
+      </c>
+      <c r="F65" t="n">
         <v>22.0</v>
       </c>
-      <c r="F65" t="n">
+      <c r="G65" t="n">
         <v>0.8461538461538461</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B66" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="C66" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="D66" t="s">
-        <v>205</v>
-      </c>
-      <c r="E66" t="n">
+        <v>270</v>
+      </c>
+      <c r="E66" t="s">
+        <v>300</v>
+      </c>
+      <c r="F66" t="n">
         <v>23.0</v>
       </c>
-      <c r="F66" t="n">
+      <c r="G66" t="n">
         <v>0.8846153846153846</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B67" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="C67" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="D67" t="s">
-        <v>205</v>
-      </c>
-      <c r="E67" t="n">
+        <v>271</v>
+      </c>
+      <c r="E67" t="s">
+        <v>300</v>
+      </c>
+      <c r="F67" t="n">
         <v>24.0</v>
       </c>
-      <c r="F67" t="n">
+      <c r="G67" t="n">
         <v>0.9230769230769231</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B68" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="C68" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="D68" t="s">
-        <v>205</v>
-      </c>
-      <c r="E68" t="n">
+        <v>272</v>
+      </c>
+      <c r="E68" t="s">
+        <v>300</v>
+      </c>
+      <c r="F68" t="n">
         <v>24.0</v>
       </c>
-      <c r="F68" t="n">
+      <c r="G68" t="n">
         <v>0.9230769230769231</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B69" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="C69" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="D69" t="s">
-        <v>205</v>
-      </c>
-      <c r="E69" t="n">
+        <v>273</v>
+      </c>
+      <c r="E69" t="s">
+        <v>300</v>
+      </c>
+      <c r="F69" t="n">
         <v>24.0</v>
       </c>
-      <c r="F69" t="n">
+      <c r="G69" t="n">
         <v>0.9230769230769231</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B70" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="C70" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="D70" t="s">
-        <v>205</v>
-      </c>
-      <c r="E70" t="n">
+        <v>274</v>
+      </c>
+      <c r="E70" t="s">
+        <v>300</v>
+      </c>
+      <c r="F70" t="n">
         <v>25.0</v>
       </c>
-      <c r="F70" t="n">
+      <c r="G70" t="n">
         <v>0.9615384615384616</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B71" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="C71" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="D71" t="s">
-        <v>205</v>
-      </c>
-      <c r="E71" t="n">
+        <v>275</v>
+      </c>
+      <c r="E71" t="s">
+        <v>300</v>
+      </c>
+      <c r="F71" t="n">
         <v>26.0</v>
       </c>
-      <c r="F71" t="n">
+      <c r="G71" t="n">
         <v>1.0</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B72" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C72" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="D72" t="s">
-        <v>205</v>
-      </c>
-      <c r="E72" t="n">
+        <v>276</v>
+      </c>
+      <c r="E72" t="s">
+        <v>300</v>
+      </c>
+      <c r="F72" t="n">
         <v>11.0</v>
       </c>
-      <c r="F72" t="n">
+      <c r="G72" t="n">
         <v>0.4230769230769231</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B73" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C73" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="D73" t="s">
-        <v>205</v>
-      </c>
-      <c r="E73" t="n">
+        <v>277</v>
+      </c>
+      <c r="E73" t="s">
+        <v>300</v>
+      </c>
+      <c r="F73" t="n">
         <v>15.0</v>
       </c>
-      <c r="F73" t="n">
+      <c r="G73" t="n">
         <v>0.5769230769230769</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B74" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C74" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="D74" t="s">
-        <v>205</v>
-      </c>
-      <c r="E74" t="n">
+        <v>278</v>
+      </c>
+      <c r="E74" t="s">
+        <v>300</v>
+      </c>
+      <c r="F74" t="n">
         <v>19.0</v>
       </c>
-      <c r="F74" t="n">
+      <c r="G74" t="n">
         <v>0.7307692307692307</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B75" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C75" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="D75" t="s">
-        <v>205</v>
-      </c>
-      <c r="E75" t="n">
+        <v>279</v>
+      </c>
+      <c r="E75" t="s">
+        <v>300</v>
+      </c>
+      <c r="F75" t="n">
         <v>21.0</v>
       </c>
-      <c r="F75" t="n">
+      <c r="G75" t="n">
         <v>0.8076923076923077</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B76" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C76" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="D76" t="s">
-        <v>205</v>
-      </c>
-      <c r="E76" t="n">
+        <v>280</v>
+      </c>
+      <c r="E76" t="s">
+        <v>300</v>
+      </c>
+      <c r="F76" t="n">
         <v>23.0</v>
       </c>
-      <c r="F76" t="n">
+      <c r="G76" t="n">
         <v>0.8846153846153846</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B77" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C77" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="D77" t="s">
-        <v>205</v>
-      </c>
-      <c r="E77" t="n">
+        <v>281</v>
+      </c>
+      <c r="E77" t="s">
+        <v>300</v>
+      </c>
+      <c r="F77" t="n">
         <v>26.0</v>
       </c>
-      <c r="F77" t="n">
+      <c r="G77" t="n">
         <v>1.0</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B78" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C78" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="D78" t="s">
-        <v>205</v>
-      </c>
-      <c r="E78" t="n">
+        <v>282</v>
+      </c>
+      <c r="E78" t="s">
+        <v>300</v>
+      </c>
+      <c r="F78" t="n">
         <v>15.0</v>
       </c>
-      <c r="F78" t="n">
+      <c r="G78" t="n">
         <v>0.625</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B79" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C79" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="D79" t="s">
-        <v>205</v>
-      </c>
-      <c r="E79" t="n">
+        <v>283</v>
+      </c>
+      <c r="E79" t="s">
+        <v>300</v>
+      </c>
+      <c r="F79" t="n">
         <v>17.0</v>
       </c>
-      <c r="F79" t="n">
+      <c r="G79" t="n">
         <v>0.7083333333333334</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B80" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C80" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="D80" t="s">
-        <v>205</v>
-      </c>
-      <c r="E80" t="n">
+        <v>284</v>
+      </c>
+      <c r="E80" t="s">
+        <v>300</v>
+      </c>
+      <c r="F80" t="n">
         <v>18.0</v>
       </c>
-      <c r="F80" t="n">
+      <c r="G80" t="n">
         <v>0.75</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B81" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C81" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="D81" t="s">
-        <v>205</v>
-      </c>
-      <c r="E81" t="n">
+        <v>285</v>
+      </c>
+      <c r="E81" t="s">
+        <v>300</v>
+      </c>
+      <c r="F81" t="n">
         <v>20.0</v>
       </c>
-      <c r="F81" t="n">
+      <c r="G81" t="n">
         <v>0.8333333333333334</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B82" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C82" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="D82" t="s">
-        <v>205</v>
-      </c>
-      <c r="E82" t="n">
+        <v>286</v>
+      </c>
+      <c r="E82" t="s">
+        <v>300</v>
+      </c>
+      <c r="F82" t="n">
         <v>22.0</v>
       </c>
-      <c r="F82" t="n">
+      <c r="G82" t="n">
         <v>0.9166666666666666</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B83" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C83" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="D83" t="s">
-        <v>205</v>
-      </c>
-      <c r="E83" t="n">
+        <v>287</v>
+      </c>
+      <c r="E83" t="s">
+        <v>300</v>
+      </c>
+      <c r="F83" t="n">
         <v>22.0</v>
       </c>
-      <c r="F83" t="n">
+      <c r="G83" t="n">
         <v>0.9166666666666666</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B84" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C84" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="D84" t="s">
-        <v>205</v>
-      </c>
-      <c r="E84" t="n">
+        <v>288</v>
+      </c>
+      <c r="E84" t="s">
+        <v>300</v>
+      </c>
+      <c r="F84" t="n">
         <v>23.0</v>
       </c>
-      <c r="F84" t="n">
+      <c r="G84" t="n">
         <v>0.9583333333333334</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B85" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C85" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="D85" t="s">
-        <v>205</v>
-      </c>
-      <c r="E85" t="n">
+        <v>289</v>
+      </c>
+      <c r="E85" t="s">
+        <v>300</v>
+      </c>
+      <c r="F85" t="n">
         <v>18.0</v>
       </c>
-      <c r="F85" t="n">
+      <c r="G85" t="n">
         <v>0.75</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B86" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C86" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="D86" t="s">
-        <v>205</v>
-      </c>
-      <c r="E86" t="n">
+        <v>290</v>
+      </c>
+      <c r="E86" t="s">
+        <v>300</v>
+      </c>
+      <c r="F86" t="n">
         <v>21.0</v>
       </c>
-      <c r="F86" t="n">
+      <c r="G86" t="n">
         <v>0.875</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B87" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C87" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="D87" t="s">
-        <v>205</v>
-      </c>
-      <c r="E87" t="n">
+        <v>291</v>
+      </c>
+      <c r="E87" t="s">
+        <v>300</v>
+      </c>
+      <c r="F87" t="n">
         <v>21.0</v>
       </c>
-      <c r="F87" t="n">
+      <c r="G87" t="n">
         <v>0.875</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B88" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C88" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="D88" t="s">
-        <v>205</v>
-      </c>
-      <c r="E88" t="n">
+        <v>292</v>
+      </c>
+      <c r="E88" t="s">
+        <v>300</v>
+      </c>
+      <c r="F88" t="n">
         <v>23.0</v>
       </c>
-      <c r="F88" t="n">
+      <c r="G88" t="n">
         <v>0.9583333333333334</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B89" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C89" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="D89" t="s">
-        <v>205</v>
-      </c>
-      <c r="E89" t="n">
+        <v>293</v>
+      </c>
+      <c r="E89" t="s">
+        <v>300</v>
+      </c>
+      <c r="F89" t="n">
         <v>5.0</v>
       </c>
-      <c r="F89" t="n">
+      <c r="G89" t="n">
         <v>0.20833333333333334</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B90" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C90" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="D90" t="s">
-        <v>205</v>
-      </c>
-      <c r="E90" t="n">
+        <v>294</v>
+      </c>
+      <c r="E90" t="s">
+        <v>300</v>
+      </c>
+      <c r="F90" t="n">
         <v>21.0</v>
       </c>
-      <c r="F90" t="n">
+      <c r="G90" t="n">
         <v>0.875</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B91" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C91" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="D91" t="s">
-        <v>205</v>
-      </c>
-      <c r="E91" t="n">
+        <v>295</v>
+      </c>
+      <c r="E91" t="s">
+        <v>300</v>
+      </c>
+      <c r="F91" t="n">
         <v>23.0</v>
       </c>
-      <c r="F91" t="n">
+      <c r="G91" t="n">
         <v>0.9583333333333334</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="B92" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C92" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="D92" t="s">
-        <v>205</v>
-      </c>
-      <c r="E92" t="n">
+        <v>296</v>
+      </c>
+      <c r="E92" t="s">
+        <v>300</v>
+      </c>
+      <c r="F92" t="n">
         <v>23.0</v>
       </c>
-      <c r="F92" t="n">
+      <c r="G92" t="n">
         <v>0.9583333333333334</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B93" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="C93" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="D93" t="s">
-        <v>205</v>
-      </c>
-      <c r="E93" t="n">
+        <v>297</v>
+      </c>
+      <c r="E93" t="s">
+        <v>300</v>
+      </c>
+      <c r="F93" t="n">
         <v>14.0</v>
       </c>
-      <c r="F93" t="n">
+      <c r="G93" t="n">
         <v>0.5833333333333334</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B94" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="C94" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="D94" t="s">
-        <v>205</v>
-      </c>
-      <c r="E94" t="n">
+        <v>298</v>
+      </c>
+      <c r="E94" t="s">
+        <v>300</v>
+      </c>
+      <c r="F94" t="n">
         <v>23.0</v>
       </c>
-      <c r="F94" t="n">
+      <c r="G94" t="n">
         <v>0.9583333333333334</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B95" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="C95" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="D95" t="s">
-        <v>205</v>
-      </c>
-      <c r="E95" t="n">
+        <v>299</v>
+      </c>
+      <c r="E95" t="s">
+        <v>300</v>
+      </c>
+      <c r="F95" t="n">
         <v>23.0</v>
       </c>
-      <c r="F95" t="n">
+      <c r="G95" t="n">
         <v>0.9583333333333334</v>
       </c>
     </row>

</xml_diff>